<commit_message>
Update sprint_3 oraz IN/OUT
Uzupełnienie w module atrial_fibr wymaganych danych odnośnie sprintu
</commit_message>
<xml_diff>
--- a/IN_OUT.xlsx
+++ b/IN_OUT.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>Zespół</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>Dane wyjściowe</t>
+  </si>
+  <si>
+    <t>interwały RR, sygnał po filtracji, QRS-onset, QRS-end, T-end, P-onset, P-end, lokalizacja R-peaks</t>
+  </si>
+  <si>
+    <t>najwyższa amplituda sygnału af, częstotliwość dominująca, początek i koniec af</t>
   </si>
 </sst>
 </file>
@@ -736,7 +742,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,8 +1139,12 @@
       <c r="C32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="2"/>
+      <c r="D32" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>

</xml_diff>

<commit_message>
update sprint3 & IN_OUT
</commit_message>
<xml_diff>
--- a/IN_OUT.xlsx
+++ b/IN_OUT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
   <si>
     <t>Zespół</t>
   </si>
@@ -296,18 +296,194 @@
   </si>
   <si>
     <t>najwyższa amplituda sygnału af, częstotliwość dominująca, początek i koniec af</t>
+  </si>
+  <si>
+    <t>Co nam moduły dostarczą :)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prosimy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> o precyzowanie przez modyły jaki będzie format danych wyjściowych DOKŁADNIE!! np. przetworzony cały sygnał - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vector&lt;double&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (czyli amplitudy kolejnych próbek), parametry jakieśtam do wyświetlenia w tabeli -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> map&lt;Qstring,double&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (gdzie Qstring to nazwa parametru a double to jego wartość), jeśli to dane do histogramu - poprosimy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vector&lt;double&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, jako wartości kolejnych słupków i jakiś </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>double</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, który będzie szerokością słupka,  jeżeli to np. wykryte załamki to poprosimy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vector&lt;double&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - czyli numery tychże próbek, dla których stwierdzono, że są załamkiem, jeżeli na wykresie ma być zaznaczony jakiś odcinek to najlepiej </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vector&lt;double&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, gdzie kolejne wartości to będzie nr próbki startowej, długość przedziału, nr kolejnej próbki startowej, długość przedziału itd. Sorry, same nazwy tego, co będzie zwracane nic nie mówią....</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -419,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -434,6 +610,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,7 +683,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,10 +715,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -562,7 +749,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -738,14 +924,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -754,7 +940,7 @@
     <col min="5" max="5" width="72.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -769,7 +955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -782,7 +968,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -793,7 +979,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -806,7 +992,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -817,7 +1003,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -830,7 +1016,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -841,7 +1027,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -851,21 +1037,25 @@
       <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="195">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -878,7 +1068,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
         <v>25</v>
@@ -889,7 +1079,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -902,7 +1092,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
         <v>30</v>
@@ -913,7 +1103,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -926,7 +1116,7 @@
       <c r="D14" s="9"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
         <v>30</v>
@@ -937,7 +1127,7 @@
       <c r="D15" s="10"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -950,7 +1140,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>37</v>
@@ -961,7 +1151,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -974,7 +1164,7 @@
       <c r="D18" s="8"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
         <v>43</v>
@@ -985,7 +1175,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -998,7 +1188,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
         <v>48</v>
@@ -1009,7 +1199,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1022,7 +1212,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
         <v>53</v>
@@ -1033,7 +1223,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
@@ -1046,7 +1236,7 @@
       <c r="D24" s="8"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
         <v>58</v>
@@ -1057,7 +1247,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
@@ -1070,7 +1260,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="5" t="s">
         <v>63</v>
@@ -1081,7 +1271,7 @@
       <c r="D27" s="7"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -1094,7 +1284,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="3"/>
       <c r="B29" s="5" t="s">
         <v>5</v>
@@ -1105,7 +1295,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>69</v>
       </c>
@@ -1118,7 +1308,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="3"/>
       <c r="B31" s="5" t="s">
         <v>71</v>
@@ -1129,7 +1319,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -1139,14 +1329,14 @@
       <c r="C32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="3"/>
       <c r="B33" s="5" t="s">
         <v>76</v>
@@ -1157,7 +1347,7 @@
       <c r="D33" s="7"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
         <v>78</v>
       </c>
@@ -1170,7 +1360,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="3"/>
       <c r="B35" s="5" t="s">
         <v>48</v>
@@ -1181,7 +1371,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -1194,7 +1384,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
         <v>84</v>
@@ -1205,7 +1395,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="4" t="s">
         <v>86</v>
       </c>
@@ -1218,7 +1408,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="3"/>
       <c r="B39" s="5" t="s">
         <v>87</v>
@@ -1231,5 +1421,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uzupelnienie sprint_planu i InOUT
</commit_message>
<xml_diff>
--- a/IN_OUT.xlsx
+++ b/IN_OUT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
   <si>
     <t>Zespół</t>
   </si>
@@ -456,12 +456,19 @@
       <t>, gdzie kolejne wartości to będzie nr próbki startowej, długość przedziału, nr kolejnej próbki startowej, długość przedziału itd. Sorry, same nazwy tego, co będzie zwracane nic nie mówią....</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">map&lt;String, dobule&gt; - 7 parametrow analizy czasowej, map&lt;String, dobule&gt; - 6 parametrow analizy czestoliwosciowej, 2x vector&lt;double&gt; - oś X i oś Y wykresu oraz naniesione na niego paremetry z analizy czestoliwosciowej
+</t>
+  </si>
+  <si>
+    <t>double - czestoliwosc probkowania, vector&lt;double&gt; - kolejne piki R z modulu R_peaks lub czas ich wystepienia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +493,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -595,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -622,6 +636,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,7 +709,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -715,9 +741,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,6 +776,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -924,14 +952,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -940,7 +968,7 @@
     <col min="5" max="5" width="72.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -955,7 +983,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -968,7 +996,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -979,7 +1007,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -992,7 +1020,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -1003,7 +1031,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1016,7 +1044,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -1027,7 +1055,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1070,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="195">
+    <row r="9" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="13" t="s">
         <v>20</v>
@@ -1055,7 +1083,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1068,7 +1096,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
         <v>25</v>
@@ -1079,7 +1107,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1092,7 +1120,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
         <v>30</v>
@@ -1103,7 +1131,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1116,7 +1144,7 @@
       <c r="D14" s="9"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
         <v>30</v>
@@ -1127,7 +1155,7 @@
       <c r="D15" s="10"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -1140,7 +1168,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>37</v>
@@ -1151,7 +1179,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1161,10 +1189,14 @@
       <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="D18" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
         <v>43</v>
@@ -1172,10 +1204,10 @@
       <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D19" s="18"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1188,7 +1220,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
         <v>48</v>
@@ -1199,7 +1231,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1212,7 +1244,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
         <v>53</v>
@@ -1223,7 +1255,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
@@ -1236,7 +1268,7 @@
       <c r="D24" s="8"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
         <v>58</v>
@@ -1247,7 +1279,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
@@ -1260,7 +1292,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="5" t="s">
         <v>63</v>
@@ -1271,7 +1303,7 @@
       <c r="D27" s="7"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -1284,7 +1316,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="5" t="s">
         <v>5</v>
@@ -1295,7 +1327,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>69</v>
       </c>
@@ -1308,7 +1340,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="5" t="s">
         <v>71</v>
@@ -1319,7 +1351,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -1336,7 +1368,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="5" t="s">
         <v>76</v>
@@ -1347,7 +1379,7 @@
       <c r="D33" s="7"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>78</v>
       </c>
@@ -1360,7 +1392,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="5" t="s">
         <v>48</v>
@@ -1371,7 +1403,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -1384,7 +1416,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
         <v>84</v>
@@ -1395,7 +1427,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>86</v>
       </c>
@@ -1408,7 +1440,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="5" t="s">
         <v>87</v>
@@ -1420,6 +1452,10 @@
       <c r="E39" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update sprintu nr3, dodanie w IN_OUT.xlsx kolumny
</commit_message>
<xml_diff>
--- a/IN_OUT.xlsx
+++ b/IN_OUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t>Zespół</t>
   </si>
@@ -469,6 +469,24 @@
   <si>
     <t>OUT: vector&lt;double&gt; - sygnał oddechowy (EDR), czyli amplituda sygnału w kolejnych wartościach próbek, wykres EDR</t>
   </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>2 tabele + wykres</t>
+  </si>
+  <si>
+    <t>wykres</t>
+  </si>
+  <si>
+    <t>Wizualizacja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT: Wskaźniki do QwtPlotów i Qwidgetów </t>
+  </si>
+  <si>
+    <t>IN: ścieżka do pliku *.hea</t>
+  </si>
 </sst>
 </file>
 
@@ -615,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -662,6 +680,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -964,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -977,9 +999,10 @@
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="66.7109375" customWidth="1"/>
     <col min="5" max="5" width="72.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -993,8 +1016,11 @@
       <c r="E1" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1033,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="3"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -1018,7 +1044,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1031,7 +1057,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -1042,7 +1068,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1052,10 +1078,12 @@
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -1063,10 +1091,12 @@
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1081,7 +1111,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="195">
+    <row r="9" spans="1:6" ht="195">
       <c r="A9" s="3"/>
       <c r="B9" s="12" t="s">
         <v>20</v>
@@ -1094,7 +1124,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1107,7 +1137,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
         <v>25</v>
@@ -1118,7 +1148,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1131,7 +1161,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
         <v>30</v>
@@ -1142,7 +1172,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1158,8 +1188,11 @@
       <c r="E14" s="20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.5" customHeight="1">
+      <c r="F14" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
         <v>30</v>
@@ -1169,8 +1202,9 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -1183,7 +1217,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>37</v>
@@ -1194,7 +1228,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1210,8 +1244,11 @@
       <c r="E18" s="14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
         <v>43</v>
@@ -1221,8 +1258,9 @@
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1235,7 +1273,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
         <v>48</v>
@@ -1246,7 +1284,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1259,7 +1297,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
         <v>53</v>
@@ -1270,7 +1308,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
@@ -1283,7 +1321,7 @@
       <c r="D24" s="8"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
         <v>58</v>
@@ -1294,7 +1332,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
@@ -1307,7 +1345,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="3"/>
       <c r="B27" s="5" t="s">
         <v>63</v>
@@ -1318,7 +1356,7 @@
       <c r="D27" s="7"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -1331,7 +1369,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="3"/>
       <c r="B29" s="5" t="s">
         <v>5</v>
@@ -1342,7 +1380,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>69</v>
       </c>
@@ -1355,7 +1393,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="3"/>
       <c r="B31" s="5" t="s">
         <v>71</v>
@@ -1366,7 +1404,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -1382,8 +1420,11 @@
       <c r="E32" s="11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3"/>
       <c r="B33" s="5" t="s">
         <v>76</v>
@@ -1393,8 +1434,9 @@
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>78</v>
       </c>
@@ -1407,7 +1449,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35" s="3"/>
       <c r="B35" s="5" t="s">
         <v>48</v>
@@ -1418,7 +1460,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -1431,7 +1473,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
         <v>84</v>
@@ -1442,7 +1484,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>86</v>
       </c>
@@ -1455,7 +1497,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="3"/>
       <c r="B39" s="5" t="s">
         <v>87</v>
@@ -1467,11 +1509,14 @@
       <c r="E39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update sprintu 3, uzupelnienie in/out
</commit_message>
<xml_diff>
--- a/IN_OUT.xlsx
+++ b/IN_OUT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
   <si>
     <t>Zespół</t>
   </si>
@@ -469,6 +469,12 @@
   <si>
     <t>map&lt;string,double&gt; najwyższa amplituda sygnału af, map&lt;string,double&gt; częstotliwość dominująca, vector&lt;double&gt; początek i koniec af</t>
   </si>
+  <si>
+    <t>Vector &lt;double&gt; od modułu I/O - nieprzefiltrowany sygnał</t>
+  </si>
+  <si>
+    <t>Vector &lt;double&gt;  - przefiltrowany sygnał z usuniętą linią bazową</t>
+  </si>
 </sst>
 </file>
 
@@ -641,6 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -656,12 +668,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,8 +1113,12 @@
       <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -1155,10 +1165,10 @@
       <c r="C14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="20" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1170,8 +1180,8 @@
       <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1207,10 +1217,10 @@
       <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="14" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1222,8 +1232,8 @@
       <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="21"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">

</xml_diff>